<commit_message>
created UGR_table in RMarkdown.
</commit_message>
<xml_diff>
--- a/CIE-190-2010_tables.xlsx
+++ b/CIE-190-2010_tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Table 2" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="63">
   <si>
     <t>gamma</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>B</t>
-  </si>
-  <si>
-    <t>SH</t>
   </si>
   <si>
     <t>F_GL1</t>
@@ -2790,8 +2787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2816,16 +2813,16 @@
         <v>17</v>
       </c>
       <c r="D1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2925,7 +2922,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C6" s="3">
         <v>1.6</v>
@@ -3274,8 +3271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:L40"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26:K40"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3286,7 +3283,7 @@
   <sheetData>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>9</v>
@@ -3321,10 +3318,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>9</v>
@@ -3359,10 +3356,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="9">
         <v>1</v>
@@ -3397,10 +3394,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="8">
         <v>0.22</v>
@@ -3435,10 +3432,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="8">
         <v>0.42199999999999999</v>
@@ -3473,10 +3470,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="8">
         <v>0.64600000000000002</v>
@@ -3511,10 +3508,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="8">
         <v>0.16600000000000001</v>
@@ -3549,10 +3546,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="8">
         <v>0.217</v>
@@ -3587,10 +3584,10 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="8">
         <v>0.55300000000000005</v>
@@ -3625,10 +3622,10 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="8">
         <v>0.19800000000000001</v>
@@ -3663,10 +3660,10 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" s="8">
         <v>0.38</v>
@@ -3701,10 +3698,10 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" s="8">
         <v>0.44500000000000001</v>
@@ -3739,10 +3736,10 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>33</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>34</v>
       </c>
       <c r="C15" s="8">
         <v>0.17199999999999999</v>
@@ -3777,10 +3774,10 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" s="8">
         <v>0.19800000000000001</v>
@@ -3815,10 +3812,10 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="8">
         <v>0.38600000000000001</v>
@@ -3853,10 +3850,10 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="8">
         <v>0.157</v>
@@ -3891,10 +3888,10 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="8">
         <v>0.18099999999999999</v>
@@ -3929,10 +3926,10 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" s="8">
         <v>0.22700000000000001</v>
@@ -3967,7 +3964,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>11</v>
@@ -3999,10 +3996,10 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>13</v>
@@ -4034,10 +4031,10 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" s="9">
         <v>2.67</v>
@@ -4069,10 +4066,10 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" s="8">
         <v>0.115</v>
@@ -4104,10 +4101,10 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27" s="8">
         <v>0.21099999999999999</v>
@@ -4139,10 +4136,10 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C28" s="8">
         <v>0.307</v>
@@ -4174,10 +4171,10 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C29" s="8">
         <v>0.106</v>
@@ -4209,10 +4206,10 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" s="8">
         <v>0.11700000000000001</v>
@@ -4244,10 +4241,10 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C31" s="8">
         <v>0.28299999999999997</v>
@@ -4279,10 +4276,10 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" s="8">
         <v>0.1</v>
@@ -4314,10 +4311,10 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" s="8">
         <v>0.187</v>
@@ -4349,10 +4346,10 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" s="8">
         <v>0.21099999999999999</v>
@@ -4384,10 +4381,10 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="10" t="s">
         <v>33</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>34</v>
       </c>
       <c r="C35" s="8">
         <v>9.2999999999999999E-2</v>
@@ -4419,10 +4416,10 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C36" s="8">
         <v>0.104</v>
@@ -4454,10 +4451,10 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C37" s="8">
         <v>0.19600000000000001</v>
@@ -4489,10 +4486,10 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C38" s="8">
         <v>8.1000000000000003E-2</v>
@@ -4524,10 +4521,10 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C39" s="8">
         <v>9.1999999999999998E-2</v>
@@ -4559,10 +4556,10 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C40" s="8">
         <v>0.114</v>
@@ -4602,7 +4599,7 @@
   <dimension ref="A1:G96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I1:AW1048576"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4618,7 +4615,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>16</v>
@@ -4627,21 +4624,21 @@
         <v>15</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>9</v>
@@ -4664,7 +4661,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>9</v>
@@ -4687,7 +4684,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>9</v>
@@ -4710,7 +4707,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>9</v>
@@ -4733,7 +4730,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>9</v>
@@ -4756,7 +4753,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>9</v>
@@ -4779,7 +4776,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>11</v>
@@ -4802,7 +4799,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>11</v>
@@ -4825,7 +4822,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="16" t="s">
         <v>11</v>
@@ -4848,7 +4845,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>11</v>
@@ -4871,7 +4868,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>11</v>
@@ -4883,18 +4880,18 @@
         <v>2.67</v>
       </c>
       <c r="E12" s="8">
-        <v>0.16600000000000001</v>
+        <v>0.115</v>
       </c>
       <c r="F12" s="8">
-        <v>0.217</v>
+        <v>0.21099999999999999</v>
       </c>
       <c r="G12" s="8">
-        <v>0.55300000000000005</v>
+        <v>0.307</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>11</v>
@@ -4906,18 +4903,18 @@
         <v>3</v>
       </c>
       <c r="E13" s="8">
-        <v>0.17299999999999999</v>
+        <v>0.105</v>
       </c>
       <c r="F13" s="8">
-        <v>0.19600000000000001</v>
+        <v>0.19</v>
       </c>
       <c r="G13" s="8">
-        <v>0.497</v>
+        <v>0.27900000000000003</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>13</v>
@@ -4929,18 +4926,18 @@
         <v>2.67</v>
       </c>
       <c r="E14" s="8">
-        <v>0.16400000000000001</v>
+        <v>0.115</v>
       </c>
       <c r="F14" s="8">
-        <v>0.184</v>
+        <v>0.21099999999999999</v>
       </c>
       <c r="G14" s="8">
-        <v>0.46500000000000002</v>
+        <v>0.307</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>13</v>
@@ -4952,18 +4949,18 @@
         <v>3.43</v>
       </c>
       <c r="E15" s="8">
-        <v>0.154</v>
+        <v>9.4E-2</v>
       </c>
       <c r="F15" s="8">
-        <v>0.17100000000000001</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="G15" s="8">
-        <v>0.432</v>
+        <v>0.247</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>13</v>
@@ -4975,18 +4972,18 @@
         <v>4</v>
       </c>
       <c r="E16" s="8">
-        <v>0.14899999999999999</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="F16" s="8">
-        <v>0.16400000000000001</v>
+        <v>0.155</v>
       </c>
       <c r="G16" s="8">
-        <v>0.41499999999999998</v>
+        <v>0.215</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>13</v>
@@ -4995,21 +4992,21 @@
         <v>14</v>
       </c>
       <c r="D17" s="18">
-        <v>4.5999999999999996</v>
+        <v>4.8</v>
       </c>
       <c r="E17" s="8">
-        <v>0.14299999999999999</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="F17" s="8">
-        <v>0.156</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="G17" s="8">
-        <v>0.39700000000000002</v>
+        <v>0.183</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" s="16" t="s">
         <v>14</v>
@@ -5021,18 +5018,18 @@
         <v>3</v>
       </c>
       <c r="E18" s="8">
-        <v>0.16400000000000001</v>
+        <v>0.105</v>
       </c>
       <c r="F18" s="8">
-        <v>0.184</v>
+        <v>0.19</v>
       </c>
       <c r="G18" s="8">
-        <v>0.46500000000000002</v>
+        <v>0.27900000000000003</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>14</v>
@@ -5044,18 +5041,18 @@
         <v>4</v>
       </c>
       <c r="E19" s="8">
-        <v>0.14199999999999999</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="F19" s="8">
-        <v>0.159</v>
+        <v>0.153</v>
       </c>
       <c r="G19" s="8">
-        <v>0.39300000000000002</v>
+        <v>0.216</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>14</v>
@@ -5067,18 +5064,18 @@
         <v>4.8</v>
       </c>
       <c r="E20" s="8">
-        <v>0.129</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="F20" s="8">
-        <v>0.14399999999999999</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="G20" s="8">
-        <v>0.35099999999999998</v>
+        <v>0.183</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>9</v>
@@ -5090,18 +5087,18 @@
         <v>1</v>
       </c>
       <c r="E21" s="8">
-        <v>0.114</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="F21" s="8">
-        <v>0.127</v>
+        <v>0.217</v>
       </c>
       <c r="G21" s="8">
-        <v>0.307</v>
+        <v>0.55300000000000005</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>9</v>
@@ -5113,18 +5110,18 @@
         <v>1.2</v>
       </c>
       <c r="E22" s="13">
-        <v>0.19800000000000001</v>
+        <v>0.17299999999999999</v>
       </c>
       <c r="F22" s="13">
-        <v>0.38</v>
+        <v>0.19600000000000001</v>
       </c>
       <c r="G22" s="13">
-        <v>0.44500000000000001</v>
+        <v>0.497</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>9</v>
@@ -5136,18 +5133,18 @@
         <v>1.33</v>
       </c>
       <c r="E23" s="13">
-        <v>0.17799999999999999</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="F23" s="13">
-        <v>0.33800000000000002</v>
+        <v>0.184</v>
       </c>
       <c r="G23" s="13">
-        <v>0.39300000000000002</v>
+        <v>0.46500000000000002</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" s="16" t="s">
         <v>9</v>
@@ -5159,18 +5156,18 @@
         <v>1.5</v>
       </c>
       <c r="E24" s="13">
-        <v>0.16600000000000001</v>
+        <v>0.154</v>
       </c>
       <c r="F24" s="13">
-        <v>0.314</v>
+        <v>0.17100000000000001</v>
       </c>
       <c r="G24" s="13">
-        <v>0.36499999999999999</v>
+        <v>0.432</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>9</v>
@@ -5182,18 +5179,18 @@
         <v>1.6</v>
       </c>
       <c r="E25" s="13">
-        <v>0.154</v>
+        <v>0.14899999999999999</v>
       </c>
       <c r="F25" s="13">
-        <v>0.28699999999999998</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="G25" s="13">
-        <v>0.33500000000000002</v>
+        <v>0.41499999999999998</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>9</v>
@@ -5205,18 +5202,18 @@
         <v>1.71</v>
       </c>
       <c r="E26" s="13">
-        <v>0.14699999999999999</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="F26" s="13">
-        <v>0.27300000000000002</v>
+        <v>0.156</v>
       </c>
       <c r="G26" s="13">
-        <v>0.32</v>
+        <v>0.39700000000000002</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27" s="16" t="s">
         <v>11</v>
@@ -5228,18 +5225,18 @@
         <v>1.33</v>
       </c>
       <c r="E27" s="13">
-        <v>0.14099999999999999</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="F27" s="13">
-        <v>0.25700000000000001</v>
+        <v>0.184</v>
       </c>
       <c r="G27" s="13">
-        <v>0.30399999999999999</v>
+        <v>0.46500000000000002</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B28" s="16" t="s">
         <v>11</v>
@@ -5251,18 +5248,18 @@
         <v>1.71</v>
       </c>
       <c r="E28" s="13">
-        <v>0.16600000000000001</v>
+        <v>0.14199999999999999</v>
       </c>
       <c r="F28" s="13">
-        <v>0.314</v>
+        <v>0.159</v>
       </c>
       <c r="G28" s="13">
-        <v>0.36399999999999999</v>
+        <v>0.39300000000000002</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="16" t="s">
         <v>11</v>
@@ -5274,18 +5271,18 @@
         <v>2</v>
       </c>
       <c r="E29" s="13">
-        <v>0.14000000000000001</v>
+        <v>0.129</v>
       </c>
       <c r="F29" s="13">
-        <v>0.26300000000000001</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="G29" s="13">
-        <v>0.30099999999999999</v>
+        <v>0.35099999999999998</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="16" t="s">
         <v>11</v>
@@ -5297,18 +5294,18 @@
         <v>2.4</v>
       </c>
       <c r="E30" s="13">
-        <v>0.125</v>
+        <v>0.114</v>
       </c>
       <c r="F30" s="13">
-        <v>0.23499999999999999</v>
+        <v>0.127</v>
       </c>
       <c r="G30" s="13">
-        <v>0.26700000000000002</v>
+        <v>0.307</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="16" t="s">
         <v>11</v>
@@ -5320,18 +5317,18 @@
         <v>2.67</v>
       </c>
       <c r="E31" s="13">
-        <v>0.108</v>
+        <v>0.106</v>
       </c>
       <c r="F31" s="13">
-        <v>0.20399999999999999</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="G31" s="13">
-        <v>0.23</v>
+        <v>0.28299999999999997</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="16" t="s">
         <v>11</v>
@@ -5343,18 +5340,18 @@
         <v>3</v>
       </c>
       <c r="E32" s="8">
-        <v>0.17199999999999999</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="F32" s="8">
-        <v>0.19800000000000001</v>
+        <v>0.106</v>
       </c>
       <c r="G32" s="8">
-        <v>0.38600000000000001</v>
+        <v>0.25900000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" s="16" t="s">
         <v>13</v>
@@ -5366,18 +5363,18 @@
         <v>2.67</v>
       </c>
       <c r="E33" s="8">
-        <v>0.157</v>
+        <v>0.106</v>
       </c>
       <c r="F33" s="8">
-        <v>0.17899999999999999</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="G33" s="8">
-        <v>0.34599999999999997</v>
+        <v>0.28299999999999997</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B34" s="16" t="s">
         <v>13</v>
@@ -5389,18 +5386,18 @@
         <v>3.43</v>
       </c>
       <c r="E34" s="8">
-        <v>0.14799999999999999</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="F34" s="8">
-        <v>0.16700000000000001</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="G34" s="8">
-        <v>0.32400000000000001</v>
+        <v>0.23100000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B35" s="16" t="s">
         <v>13</v>
@@ -5412,18 +5409,18 @@
         <v>4</v>
       </c>
       <c r="E35" s="8">
-        <v>0.13600000000000001</v>
+        <v>7.8E-2</v>
       </c>
       <c r="F35" s="8">
-        <v>0.155</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="G35" s="8">
-        <v>0.30099999999999999</v>
+        <v>0.20300000000000001</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B36" s="16" t="s">
         <v>13</v>
@@ -5432,21 +5429,21 @@
         <v>14</v>
       </c>
       <c r="D36" s="18">
-        <v>4.5999999999999996</v>
+        <v>4.8</v>
       </c>
       <c r="E36" s="8">
-        <v>0.13300000000000001</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="F36" s="8">
-        <v>0.14699999999999999</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="G36" s="8">
-        <v>0.28799999999999998</v>
+        <v>0.17399999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B37" s="16" t="s">
         <v>14</v>
@@ -5458,18 +5455,18 @@
         <v>3</v>
       </c>
       <c r="E37" s="8">
-        <v>0.128</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="F37" s="8">
-        <v>0.14000000000000001</v>
+        <v>0.106</v>
       </c>
       <c r="G37" s="8">
-        <v>0.27600000000000002</v>
+        <v>0.25900000000000001</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B38" s="16" t="s">
         <v>14</v>
@@ -5481,18 +5478,18 @@
         <v>4</v>
       </c>
       <c r="E38" s="8">
-        <v>0.14799999999999999</v>
+        <v>7.8E-2</v>
       </c>
       <c r="F38" s="8">
-        <v>0.16700000000000001</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="G38" s="8">
-        <v>0.32400000000000001</v>
+        <v>0.20399999999999999</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B39" s="16" t="s">
         <v>14</v>
@@ -5504,18 +5501,18 @@
         <v>4.8</v>
       </c>
       <c r="E39" s="8">
-        <v>0.126</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="F39" s="8">
-        <v>0.14299999999999999</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="G39" s="8">
-        <v>0.27200000000000002</v>
+        <v>0.17399999999999999</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B40" s="16" t="s">
         <v>9</v>
@@ -5527,18 +5524,18 @@
         <v>1</v>
       </c>
       <c r="E40" s="8">
-        <v>0.114</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="F40" s="8">
-        <v>0.129</v>
+        <v>0.38</v>
       </c>
       <c r="G40" s="8">
-        <v>0.24399999999999999</v>
+        <v>0.44500000000000001</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B41" s="16" t="s">
         <v>9</v>
@@ -5550,18 +5547,18 @@
         <v>1.2</v>
       </c>
       <c r="E41" s="8">
-        <v>0.1</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="F41" s="8">
-        <v>0.113</v>
+        <v>0.33800000000000002</v>
       </c>
       <c r="G41" s="8">
-        <v>0.21199999999999999</v>
+        <v>0.39300000000000002</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B42" s="16" t="s">
         <v>9</v>
@@ -5573,18 +5570,18 @@
         <v>1.33</v>
       </c>
       <c r="E42" s="8">
-        <v>0.157</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="F42" s="8">
-        <v>0.18099999999999999</v>
+        <v>0.314</v>
       </c>
       <c r="G42" s="8">
-        <v>0.22700000000000001</v>
+        <v>0.36499999999999999</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B43" s="16" t="s">
         <v>9</v>
@@ -5596,18 +5593,18 @@
         <v>1.5</v>
       </c>
       <c r="E43" s="8">
-        <v>0.14099999999999999</v>
+        <v>0.154</v>
       </c>
       <c r="F43" s="8">
-        <v>0.16200000000000001</v>
+        <v>0.28699999999999998</v>
       </c>
       <c r="G43" s="8">
-        <v>0.20300000000000001</v>
+        <v>0.33500000000000002</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B44" s="16" t="s">
         <v>9</v>
@@ -5619,18 +5616,18 @@
         <v>1.6</v>
       </c>
       <c r="E44" s="8">
-        <v>0.13200000000000001</v>
+        <v>0.14699999999999999</v>
       </c>
       <c r="F44" s="8">
-        <v>0.151</v>
+        <v>0.27300000000000002</v>
       </c>
       <c r="G44" s="8">
-        <v>0.19</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B45" s="16" t="s">
         <v>9</v>
@@ -5642,18 +5639,18 @@
         <v>1.71</v>
       </c>
       <c r="E45" s="8">
-        <v>0.123</v>
+        <v>0.14099999999999999</v>
       </c>
       <c r="F45" s="8">
-        <v>0.13900000000000001</v>
+        <v>0.25700000000000001</v>
       </c>
       <c r="G45" s="8">
-        <v>0.17599999999999999</v>
+        <v>0.30399999999999999</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B46" s="16" t="s">
         <v>11</v>
@@ -5665,18 +5662,18 @@
         <v>1.33</v>
       </c>
       <c r="E46" s="8">
-        <v>0.11799999999999999</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="F46" s="8">
-        <v>0.13200000000000001</v>
+        <v>0.314</v>
       </c>
       <c r="G46" s="8">
-        <v>0.16900000000000001</v>
+        <v>0.36399999999999999</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B47" s="16" t="s">
         <v>11</v>
@@ -5688,18 +5685,18 @@
         <v>1.71</v>
       </c>
       <c r="E47" s="8">
-        <v>0.113</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F47" s="8">
-        <v>0.124</v>
+        <v>0.26300000000000001</v>
       </c>
       <c r="G47" s="8">
-        <v>0.161</v>
+        <v>0.30099999999999999</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B48" s="16" t="s">
         <v>11</v>
@@ -5711,18 +5708,18 @@
         <v>2</v>
       </c>
       <c r="E48" s="8">
-        <v>0.13200000000000001</v>
+        <v>0.125</v>
       </c>
       <c r="F48" s="8">
-        <v>0.151</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="G48" s="8">
-        <v>0.19</v>
+        <v>0.26700000000000002</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B49" s="16" t="s">
         <v>11</v>
@@ -5734,18 +5731,18 @@
         <v>2.4</v>
       </c>
       <c r="E49" s="8">
-        <v>0.112</v>
+        <v>0.108</v>
       </c>
       <c r="F49" s="8">
-        <v>0.128</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="G49" s="8">
-        <v>0.159</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B50" s="16" t="s">
         <v>11</v>
@@ -5760,15 +5757,15 @@
         <v>0.1</v>
       </c>
       <c r="F50" s="8">
-        <v>0.115</v>
+        <v>0.187</v>
       </c>
       <c r="G50" s="8">
-        <v>0.14199999999999999</v>
+        <v>0.21099999999999999</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B51" s="16" t="s">
         <v>11</v>
@@ -5780,18 +5777,18 @@
         <v>3</v>
       </c>
       <c r="E51" s="8">
-        <v>8.6999999999999994E-2</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="F51" s="8">
-        <v>0.10100000000000001</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="G51" s="8">
-        <v>0.124</v>
+        <v>0.191</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B52" s="16" t="s">
         <v>13</v>
@@ -5803,18 +5800,18 @@
         <v>2.67</v>
       </c>
       <c r="E52" s="8">
-        <v>0.115</v>
+        <v>0.1</v>
       </c>
       <c r="F52" s="8">
+        <v>0.187</v>
+      </c>
+      <c r="G52" s="8">
         <v>0.21099999999999999</v>
-      </c>
-      <c r="G52" s="8">
-        <v>0.307</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B53" s="16" t="s">
         <v>13</v>
@@ -5826,18 +5823,18 @@
         <v>3.43</v>
       </c>
       <c r="E53" s="8">
-        <v>0.105</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="F53" s="8">
-        <v>0.19</v>
+        <v>0.154</v>
       </c>
       <c r="G53" s="8">
-        <v>0.27900000000000003</v>
+        <v>0.16900000000000001</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B54" s="16" t="s">
         <v>13</v>
@@ -5849,18 +5846,18 @@
         <v>4</v>
       </c>
       <c r="E54" s="8">
-        <v>0.115</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="F54" s="8">
-        <v>0.21099999999999999</v>
+        <v>0.13700000000000001</v>
       </c>
       <c r="G54" s="8">
-        <v>0.307</v>
+        <v>0.14699999999999999</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B55" s="16" t="s">
         <v>13</v>
@@ -5869,21 +5866,21 @@
         <v>14</v>
       </c>
       <c r="D55" s="18">
-        <v>4.5999999999999996</v>
+        <v>4.8</v>
       </c>
       <c r="E55" s="8">
-        <v>9.4E-2</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="F55" s="8">
-        <v>0.17499999999999999</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="G55" s="8">
-        <v>0.247</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B56" s="16" t="s">
         <v>14</v>
@@ -5895,18 +5892,18 @@
         <v>3</v>
       </c>
       <c r="E56" s="8">
-        <v>8.3000000000000004E-2</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="F56" s="8">
-        <v>0.155</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="G56" s="8">
-        <v>0.215</v>
+        <v>0.191</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B57" s="16" t="s">
         <v>14</v>
@@ -5921,15 +5918,15 @@
         <v>7.0999999999999994E-2</v>
       </c>
       <c r="F57" s="8">
-        <v>0.13300000000000001</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="G57" s="8">
-        <v>0.183</v>
+        <v>0.14799999999999999</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B58" s="16" t="s">
         <v>14</v>
@@ -5941,18 +5938,18 @@
         <v>4.8</v>
       </c>
       <c r="E58" s="8">
-        <v>0.105</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="F58" s="8">
-        <v>0.19</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="G58" s="8">
-        <v>0.27900000000000003</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B59" s="16" t="s">
         <v>9</v>
@@ -5964,18 +5961,18 @@
         <v>1</v>
       </c>
       <c r="E59" s="8">
-        <v>8.3000000000000004E-2</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="F59" s="8">
-        <v>0.153</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="G59" s="8">
-        <v>0.216</v>
+        <v>0.38600000000000001</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B60" s="16" t="s">
         <v>9</v>
@@ -5987,18 +5984,18 @@
         <v>1.2</v>
       </c>
       <c r="E60" s="8">
-        <v>7.0999999999999994E-2</v>
+        <v>0.157</v>
       </c>
       <c r="F60" s="8">
-        <v>0.13300000000000001</v>
+        <v>0.17899999999999999</v>
       </c>
       <c r="G60" s="8">
-        <v>0.183</v>
+        <v>0.34599999999999997</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B61" s="16" t="s">
         <v>9</v>
@@ -6010,18 +6007,18 @@
         <v>1.33</v>
       </c>
       <c r="E61" s="8">
-        <v>0.106</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="F61" s="8">
-        <v>0.11700000000000001</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="G61" s="8">
-        <v>0.28299999999999997</v>
+        <v>0.32400000000000001</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B62" s="16" t="s">
         <v>9</v>
@@ -6033,18 +6030,18 @@
         <v>1.5</v>
       </c>
       <c r="E62" s="8">
-        <v>9.8000000000000004E-2</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="F62" s="8">
-        <v>0.106</v>
+        <v>0.155</v>
       </c>
       <c r="G62" s="8">
-        <v>0.25900000000000001</v>
+        <v>0.30099999999999999</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B63" s="16" t="s">
         <v>9</v>
@@ -6056,18 +6053,18 @@
         <v>1.6</v>
       </c>
       <c r="E63" s="8">
-        <v>0.106</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="F63" s="8">
-        <v>0.11700000000000001</v>
+        <v>0.14699999999999999</v>
       </c>
       <c r="G63" s="8">
-        <v>0.28299999999999997</v>
+        <v>0.28799999999999998</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B64" s="16" t="s">
         <v>9</v>
@@ -6079,18 +6076,18 @@
         <v>1.71</v>
       </c>
       <c r="E64" s="8">
-        <v>8.7999999999999995E-2</v>
+        <v>0.128</v>
       </c>
       <c r="F64" s="8">
-        <v>9.8000000000000004E-2</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="G64" s="8">
-        <v>0.23100000000000001</v>
+        <v>0.27600000000000002</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B65" s="16" t="s">
         <v>11</v>
@@ -6102,18 +6099,18 @@
         <v>1.33</v>
       </c>
       <c r="E65" s="8">
-        <v>7.8E-2</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="F65" s="8">
-        <v>8.7999999999999995E-2</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="G65" s="8">
-        <v>0.20300000000000001</v>
+        <v>0.32400000000000001</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B66" s="16" t="s">
         <v>11</v>
@@ -6125,18 +6122,18 @@
         <v>1.71</v>
       </c>
       <c r="E66" s="8">
-        <v>6.7000000000000004E-2</v>
+        <v>0.126</v>
       </c>
       <c r="F66" s="8">
-        <v>7.5999999999999998E-2</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="G66" s="8">
-        <v>0.17399999999999999</v>
+        <v>0.27200000000000002</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B67" s="16" t="s">
         <v>11</v>
@@ -6148,18 +6145,18 @@
         <v>2</v>
       </c>
       <c r="E67" s="8">
-        <v>9.8000000000000004E-2</v>
+        <v>0.114</v>
       </c>
       <c r="F67" s="8">
-        <v>0.106</v>
+        <v>0.129</v>
       </c>
       <c r="G67" s="8">
-        <v>0.25900000000000001</v>
+        <v>0.24399999999999999</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B68" s="16" t="s">
         <v>11</v>
@@ -6171,18 +6168,18 @@
         <v>2.4</v>
       </c>
       <c r="E68" s="8">
-        <v>7.8E-2</v>
+        <v>0.1</v>
       </c>
       <c r="F68" s="8">
-        <v>8.5999999999999993E-2</v>
+        <v>0.113</v>
       </c>
       <c r="G68" s="8">
-        <v>0.20399999999999999</v>
+        <v>0.21199999999999999</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B69" s="16" t="s">
         <v>11</v>
@@ -6194,18 +6191,18 @@
         <v>2.67</v>
       </c>
       <c r="E69" s="8">
-        <v>6.7000000000000004E-2</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="F69" s="8">
-        <v>7.5999999999999998E-2</v>
+        <v>0.104</v>
       </c>
       <c r="G69" s="8">
-        <v>0.17399999999999999</v>
+        <v>0.19600000000000001</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B70" s="16" t="s">
         <v>11</v>
@@ -6217,18 +6214,18 @@
         <v>3</v>
       </c>
       <c r="E70" s="8">
-        <v>0.1</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="F70" s="8">
-        <v>0.187</v>
+        <v>9.4E-2</v>
       </c>
       <c r="G70" s="8">
-        <v>0.21099999999999999</v>
+        <v>0.17899999999999999</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B71" s="16" t="s">
         <v>13</v>
@@ -6240,18 +6237,18 @@
         <v>2.67</v>
       </c>
       <c r="E71" s="8">
-        <v>9.0999999999999998E-2</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="F71" s="8">
-        <v>0.16700000000000001</v>
+        <v>0.104</v>
       </c>
       <c r="G71" s="8">
-        <v>0.191</v>
+        <v>0.19600000000000001</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B72" s="16" t="s">
         <v>13</v>
@@ -6263,18 +6260,18 @@
         <v>3.43</v>
       </c>
       <c r="E72" s="8">
-        <v>0.1</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="F72" s="8">
-        <v>0.187</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="G72" s="8">
-        <v>0.21099999999999999</v>
+        <v>0.158</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B73" s="16" t="s">
         <v>13</v>
@@ -6286,18 +6283,18 @@
         <v>4</v>
       </c>
       <c r="E73" s="8">
-        <v>8.1000000000000003E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="F73" s="8">
-        <v>0.154</v>
+        <v>7.8E-2</v>
       </c>
       <c r="G73" s="8">
-        <v>0.16900000000000001</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B74" s="16" t="s">
         <v>13</v>
@@ -6306,21 +6303,21 @@
         <v>14</v>
       </c>
       <c r="D74" s="18">
-        <v>4.5999999999999996</v>
+        <v>4.8</v>
       </c>
       <c r="E74" s="8">
-        <v>7.0999999999999994E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="F74" s="8">
-        <v>0.13700000000000001</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="G74" s="8">
-        <v>0.14699999999999999</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B75" s="16" t="s">
         <v>14</v>
@@ -6332,18 +6329,18 @@
         <v>3</v>
       </c>
       <c r="E75" s="8">
-        <v>6.0999999999999999E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="F75" s="8">
-        <v>0.11700000000000001</v>
+        <v>9.4E-2</v>
       </c>
       <c r="G75" s="8">
-        <v>0.125</v>
+        <v>0.17899999999999999</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B76" s="16" t="s">
         <v>14</v>
@@ -6355,18 +6352,18 @@
         <v>4</v>
       </c>
       <c r="E76" s="8">
-        <v>9.0999999999999998E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="F76" s="8">
-        <v>0.16700000000000001</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="G76" s="8">
-        <v>0.191</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B77" s="16" t="s">
         <v>14</v>
@@ -6378,18 +6375,18 @@
         <v>4.8</v>
       </c>
       <c r="E77" s="8">
-        <v>7.0999999999999994E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="F77" s="8">
-        <v>0.13400000000000001</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="G77" s="8">
-        <v>0.14799999999999999</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B78" s="16" t="s">
         <v>9</v>
@@ -6401,18 +6398,18 @@
         <v>1</v>
       </c>
       <c r="E78" s="8">
-        <v>6.0999999999999999E-2</v>
+        <v>0.157</v>
       </c>
       <c r="F78" s="8">
-        <v>0.11700000000000001</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="G78" s="8">
-        <v>0.125</v>
+        <v>0.22700000000000001</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B79" s="16" t="s">
         <v>9</v>
@@ -6424,18 +6421,18 @@
         <v>1.2</v>
       </c>
       <c r="E79" s="8">
-        <v>9.2999999999999999E-2</v>
+        <v>0.14099999999999999</v>
       </c>
       <c r="F79" s="8">
-        <v>0.104</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="G79" s="8">
-        <v>0.19600000000000001</v>
+        <v>0.20300000000000001</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B80" s="16" t="s">
         <v>9</v>
@@ -6447,18 +6444,18 @@
         <v>1.33</v>
       </c>
       <c r="E80" s="8">
-        <v>8.5000000000000006E-2</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="F80" s="8">
-        <v>9.4E-2</v>
+        <v>0.151</v>
       </c>
       <c r="G80" s="8">
-        <v>0.17899999999999999</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B81" s="16" t="s">
         <v>9</v>
@@ -6470,18 +6467,18 @@
         <v>1.5</v>
       </c>
       <c r="E81" s="8">
-        <v>9.2999999999999999E-2</v>
+        <v>0.123</v>
       </c>
       <c r="F81" s="8">
-        <v>0.104</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="G81" s="8">
-        <v>0.19600000000000001</v>
+        <v>0.17599999999999999</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B82" s="16" t="s">
         <v>9</v>
@@ -6493,18 +6490,18 @@
         <v>1.6</v>
       </c>
       <c r="E82" s="8">
-        <v>7.5999999999999998E-2</v>
+        <v>0.11799999999999999</v>
       </c>
       <c r="F82" s="8">
-        <v>8.6999999999999994E-2</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="G82" s="8">
-        <v>0.158</v>
+        <v>0.16900000000000001</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B83" s="16" t="s">
         <v>9</v>
@@ -6516,18 +6513,18 @@
         <v>1.71</v>
       </c>
       <c r="E83" s="8">
-        <v>6.7000000000000004E-2</v>
+        <v>0.113</v>
       </c>
       <c r="F83" s="8">
-        <v>7.8E-2</v>
+        <v>0.124</v>
       </c>
       <c r="G83" s="8">
-        <v>0.14000000000000001</v>
+        <v>0.161</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B84" s="16" t="s">
         <v>11</v>
@@ -6539,18 +6536,18 @@
         <v>1.33</v>
       </c>
       <c r="E84" s="8">
-        <v>5.8000000000000003E-2</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="F84" s="8">
-        <v>6.7000000000000004E-2</v>
+        <v>0.151</v>
       </c>
       <c r="G84" s="8">
-        <v>0.12</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B85" s="16" t="s">
         <v>11</v>
@@ -6562,18 +6559,18 @@
         <v>1.71</v>
       </c>
       <c r="E85" s="8">
-        <v>8.5000000000000006E-2</v>
+        <v>0.112</v>
       </c>
       <c r="F85" s="8">
-        <v>9.4E-2</v>
+        <v>0.128</v>
       </c>
       <c r="G85" s="8">
-        <v>0.17899999999999999</v>
+        <v>0.159</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B86" s="16" t="s">
         <v>11</v>
@@ -6585,18 +6582,18 @@
         <v>2</v>
       </c>
       <c r="E86" s="8">
-        <v>6.8000000000000005E-2</v>
+        <v>0.1</v>
       </c>
       <c r="F86" s="8">
-        <v>7.6999999999999999E-2</v>
+        <v>0.115</v>
       </c>
       <c r="G86" s="8">
-        <v>0.14000000000000001</v>
+        <v>0.14199999999999999</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B87" s="16" t="s">
         <v>11</v>
@@ -6608,18 +6605,18 @@
         <v>2.4</v>
       </c>
       <c r="E87" s="8">
-        <v>5.8000000000000003E-2</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="F87" s="8">
-        <v>6.7000000000000004E-2</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="G87" s="8">
-        <v>0.12</v>
+        <v>0.124</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B88" s="16" t="s">
         <v>11</v>
@@ -6642,7 +6639,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B89" s="16" t="s">
         <v>11</v>
@@ -6665,7 +6662,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B90" s="16" t="s">
         <v>13</v>
@@ -6688,7 +6685,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B91" s="16" t="s">
         <v>13</v>
@@ -6711,7 +6708,7 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B92" s="16" t="s">
         <v>13</v>
@@ -6734,7 +6731,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B93" s="16" t="s">
         <v>13</v>
@@ -6743,7 +6740,7 @@
         <v>14</v>
       </c>
       <c r="D93" s="18">
-        <v>4.5999999999999996</v>
+        <v>4.8</v>
       </c>
       <c r="E93" s="8">
         <v>4.9000000000000002E-2</v>
@@ -6757,7 +6754,7 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B94" s="16" t="s">
         <v>14</v>
@@ -6780,7 +6777,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B95" s="16" t="s">
         <v>14</v>
@@ -6803,7 +6800,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B96" s="16" t="s">
         <v>14</v>
@@ -6833,7 +6830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:Y2"/>
     </sheetView>
   </sheetViews>
@@ -6849,76 +6846,76 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">

</xml_diff>